<commit_message>
add voice list in excel file
</commit_message>
<xml_diff>
--- a/THT-Face/doc/CMD list of Face attendence .xlsx
+++ b/THT-Face/doc/CMD list of Face attendence .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\THT-Face\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1C0390-F75E-40F6-8CA7-530FBEDB9029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E6FBD4-FD17-4449-9330-39276FC9E4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28920" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$56:$F$87</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$79:$F$110</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="262">
   <si>
     <t>ping</t>
   </si>
@@ -1569,9 +1569,6 @@
     <t>0xFFFF</t>
   </si>
   <si>
-    <t>Music no</t>
-  </si>
-  <si>
     <t>Welcome</t>
   </si>
   <si>
@@ -1582,6 +1579,57 @@
   </si>
   <si>
     <t>Voice</t>
+  </si>
+  <si>
+    <t>Enrolment start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duplicate person </t>
+  </si>
+  <si>
+    <t>Enrolment Time out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device binding succesfull </t>
+  </si>
+  <si>
+    <t>Connecting to wifi</t>
+  </si>
+  <si>
+    <t>wifi connected</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>our THT company</t>
+  </si>
+  <si>
+    <t>Enrolment</t>
+  </si>
+  <si>
+    <t>Time out</t>
+  </si>
+  <si>
+    <t>Connecting</t>
+  </si>
+  <si>
+    <t>connected</t>
+  </si>
+  <si>
+    <t>wifi</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Music No</t>
+  </si>
+  <si>
+    <t>Voice No</t>
+  </si>
+  <si>
+    <t>Start</t>
   </si>
 </sst>
 </file>
@@ -1737,7 +1785,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1849,6 +1897,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1994,7 +2048,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2164,6 +2218,120 @@
     <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2185,9 +2353,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2197,9 +2362,6 @@
     <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2230,113 +2392,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2681,10 +2747,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N125"/>
+  <dimension ref="A1:N148"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2706,28 +2772,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="115" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
     </row>
     <row r="4" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="122" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="86"/>
+      <c r="B4" s="123"/>
     </row>
     <row r="5" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
@@ -2763,1395 +2829,1563 @@
     </row>
     <row r="9" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:6" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="134" t="s">
+      <c r="A10" s="79" t="s">
+        <v>260</v>
+      </c>
+      <c r="B10" s="79" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="77">
+        <v>1</v>
+      </c>
+      <c r="B11" s="78" t="s">
         <v>241</v>
       </c>
-      <c r="B10" s="134" t="s">
+    </row>
+    <row r="12" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="77">
+        <v>2</v>
+      </c>
+      <c r="B12" s="78" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="77">
+        <v>3</v>
+      </c>
+      <c r="B13" s="78" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="77">
+        <v>4</v>
+      </c>
+      <c r="B14" s="78" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="132">
+    <row r="15" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="77">
+        <v>5</v>
+      </c>
+      <c r="B15" s="78" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="77">
+        <v>6</v>
+      </c>
+      <c r="B16" s="78" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="77">
+        <v>7</v>
+      </c>
+      <c r="B17" s="78" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="77">
+        <v>8</v>
+      </c>
+      <c r="B18" s="78" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="77">
+        <v>9</v>
+      </c>
+      <c r="B19" s="78" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="135"/>
+      <c r="B20" s="136"/>
+    </row>
+    <row r="21" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="135"/>
+      <c r="B21" s="136"/>
+    </row>
+    <row r="22" spans="1:2" s="42" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="79" t="s">
+        <v>259</v>
+      </c>
+      <c r="B22" s="79" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="137">
         <v>1</v>
       </c>
-      <c r="B11" s="133" t="s">
+      <c r="B23" s="138" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="137">
+        <v>2</v>
+      </c>
+      <c r="B24" s="138" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="132">
+    <row r="25" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="137">
+        <v>3</v>
+      </c>
+      <c r="B25" s="138" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="137">
+        <v>4</v>
+      </c>
+      <c r="B26" s="138" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="137">
+        <v>5</v>
+      </c>
+      <c r="B27" s="138" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="137">
+        <v>6</v>
+      </c>
+      <c r="B28" s="138" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="137">
+        <v>7</v>
+      </c>
+      <c r="B29" s="138" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="137">
+        <v>8</v>
+      </c>
+      <c r="B30" s="138" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="137">
+        <v>9</v>
+      </c>
+      <c r="B31" s="138" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="137">
+        <v>10</v>
+      </c>
+      <c r="B32" s="138" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="137">
+        <v>11</v>
+      </c>
+      <c r="B33" s="138" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="137">
+        <v>12</v>
+      </c>
+      <c r="B34" s="138" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="135"/>
+      <c r="B35" s="136"/>
+    </row>
+    <row r="36" spans="1:5" s="42" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="135"/>
+      <c r="B36" s="136"/>
+    </row>
+    <row r="37" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="122" t="s">
+        <v>227</v>
+      </c>
+      <c r="B38" s="123"/>
+      <c r="C38" s="56" t="s">
+        <v>235</v>
+      </c>
+      <c r="D38" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" s="67"/>
+    </row>
+    <row r="39" spans="1:5" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="81" t="s">
+        <v>238</v>
+      </c>
+      <c r="B39" s="81"/>
+      <c r="C39" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="D39" s="57" t="s">
+        <v>226</v>
+      </c>
+      <c r="E39" s="68"/>
+    </row>
+    <row r="40" spans="1:5" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="81"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="61" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="E40" s="68"/>
+    </row>
+    <row r="41" spans="1:5" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="81"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="63" t="s">
+        <v>233</v>
+      </c>
+      <c r="D41" s="64" t="s">
+        <v>230</v>
+      </c>
+      <c r="E41" s="68"/>
+    </row>
+    <row r="42" spans="1:5" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="81"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="65" t="s">
+        <v>236</v>
+      </c>
+      <c r="D42" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="E42" s="68"/>
+    </row>
+    <row r="43" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="81"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="66" t="s">
+        <v>237</v>
+      </c>
+      <c r="D43" s="60" t="s">
+        <v>225</v>
+      </c>
+      <c r="E43" s="68"/>
+    </row>
+    <row r="44" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="70"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="68"/>
+    </row>
+    <row r="45" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="83"/>
+      <c r="C45" s="83"/>
+      <c r="D45" s="82" t="s">
+        <v>179</v>
+      </c>
+      <c r="E45" s="82"/>
+    </row>
+    <row r="46" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B46" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="E46" s="41" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D47" s="84" t="s">
+        <v>166</v>
+      </c>
+      <c r="E47" s="84" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" s="84"/>
+      <c r="E48" s="84"/>
+    </row>
+    <row r="49" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="5">
+        <v>45575.507002314815</v>
+      </c>
+      <c r="C49" s="39"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="84"/>
+    </row>
+    <row r="50" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" s="84"/>
+      <c r="E50" s="84"/>
+    </row>
+    <row r="51" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="84"/>
+      <c r="E51" s="84"/>
+    </row>
+    <row r="52" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="84"/>
+      <c r="E52" s="84"/>
+    </row>
+    <row r="53" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="4">
+        <v>11000</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="84"/>
+      <c r="E53" s="84"/>
+    </row>
+    <row r="54" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" s="4">
+        <v>100</v>
+      </c>
+      <c r="C54" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+    </row>
+    <row r="55" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="4">
+        <v>110</v>
+      </c>
+      <c r="C55" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="84"/>
+      <c r="E55" s="84"/>
+    </row>
+    <row r="56" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="4">
+        <v>11</v>
+      </c>
+      <c r="C56" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="84"/>
+      <c r="E56" s="84"/>
+    </row>
+    <row r="57" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="85" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="87" t="s">
+        <v>210</v>
+      </c>
+      <c r="C57" s="88"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="84"/>
+    </row>
+    <row r="58" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="86"/>
+      <c r="B58" s="89" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="90"/>
+      <c r="D58" s="84"/>
+      <c r="E58" s="84"/>
+    </row>
+    <row r="59" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="D59" s="84"/>
+      <c r="E59" s="84"/>
+    </row>
+    <row r="60" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D60" s="84"/>
+      <c r="E60" s="84"/>
+    </row>
+    <row r="61" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B61" s="4">
+        <v>6</v>
+      </c>
+      <c r="C61" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="D61" s="84"/>
+      <c r="E61" s="84"/>
+    </row>
+    <row r="62" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="4">
+        <v>10</v>
+      </c>
+      <c r="C62" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" s="84"/>
+      <c r="E62" s="84"/>
+    </row>
+    <row r="63" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B63" s="91" t="s">
+        <v>229</v>
+      </c>
+      <c r="C63" s="91"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+    </row>
+    <row r="64" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="70"/>
+      <c r="B64" s="70"/>
+      <c r="C64" s="69"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="68"/>
+    </row>
+    <row r="65" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="96" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="96"/>
+      <c r="C65" s="96"/>
+      <c r="D65" s="96"/>
+      <c r="E65" s="96"/>
+      <c r="F65" s="96"/>
+    </row>
+    <row r="66" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="124" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67" s="94"/>
+      <c r="C67" s="94"/>
+      <c r="D67" s="94"/>
+      <c r="E67" s="94"/>
+    </row>
+    <row r="68" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="D68" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E68" s="33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="B69" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C69" s="130"/>
+      <c r="D69" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="E69" s="127" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="C70" s="132"/>
+      <c r="D70" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E70" s="128"/>
+    </row>
+    <row r="71" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="B71" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="C71" s="132"/>
+      <c r="D71" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="E71" s="128"/>
+    </row>
+    <row r="72" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C72" s="132"/>
+      <c r="D72" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="E72" s="128"/>
+    </row>
+    <row r="73" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="B73" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C73" s="132"/>
+      <c r="D73" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="E73" s="128"/>
+    </row>
+    <row r="74" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="52" t="s">
+        <v>207</v>
+      </c>
+      <c r="B74" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="C74" s="131"/>
+      <c r="D74" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="E74" s="129"/>
+    </row>
+    <row r="75" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B75" s="130"/>
+      <c r="C75" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="D75" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="E75" s="125" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="43" t="s">
+        <v>205</v>
+      </c>
+      <c r="B76" s="131"/>
+      <c r="C76" s="54" t="s">
+        <v>204</v>
+      </c>
+      <c r="D76" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="E76" s="126"/>
+    </row>
+    <row r="78" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="94" t="s">
+        <v>178</v>
+      </c>
+      <c r="B78" s="94"/>
+      <c r="C78" s="94"/>
+      <c r="D78" s="94"/>
+      <c r="E78" s="94"/>
+      <c r="F78" s="94"/>
+    </row>
+    <row r="79" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A79" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="B79" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="133" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="132">
+      <c r="C79" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D79" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="E79" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="F79" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="G79" s="6"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+    </row>
+    <row r="80" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="133" t="s">
+        <v>128</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G80" s="6"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+    </row>
+    <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="133"/>
+      <c r="B81" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F81" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G81" s="6"/>
+    </row>
+    <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="133"/>
+      <c r="B82" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D82" s="9"/>
+      <c r="E82" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F82" s="12"/>
+      <c r="G82" s="6"/>
+    </row>
+    <row r="83" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="133"/>
+      <c r="B83" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F83" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G83" s="6"/>
+    </row>
+    <row r="84" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="133"/>
+      <c r="B84" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="G84" s="6"/>
+    </row>
+    <row r="85" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="133"/>
+      <c r="B85" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F85" s="9"/>
+      <c r="G85" s="6"/>
+    </row>
+    <row r="86" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="133"/>
+      <c r="B86" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F86" s="9"/>
+      <c r="G86" s="6"/>
+    </row>
+    <row r="87" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="133"/>
+      <c r="B87" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F87" s="9"/>
+      <c r="G87" s="6"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="133"/>
+      <c r="B88" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="6"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="133"/>
+      <c r="B89" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="133"/>
+      <c r="B90" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G90" s="6"/>
+    </row>
+    <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="116"/>
+      <c r="B91" s="117"/>
+      <c r="C91" s="117"/>
+      <c r="D91" s="117"/>
+      <c r="E91" s="117"/>
+      <c r="F91" s="118"/>
+      <c r="G91" s="6"/>
+    </row>
+    <row r="92" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="134" t="s">
+        <v>127</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E92" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92" s="6"/>
+    </row>
+    <row r="93" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="134"/>
+      <c r="B93" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G93" s="6"/>
+    </row>
+    <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="134"/>
+      <c r="B94" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="6"/>
+    </row>
+    <row r="95" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="134"/>
+      <c r="B95" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" s="7"/>
+      <c r="D95" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F95" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G95" s="6"/>
+    </row>
+    <row r="96" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="116"/>
+      <c r="B96" s="117"/>
+      <c r="C96" s="117"/>
+      <c r="D96" s="117"/>
+      <c r="E96" s="117"/>
+      <c r="F96" s="118"/>
+      <c r="G96" s="6"/>
+    </row>
+    <row r="97" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A97" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" s="14"/>
+      <c r="D97" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E97" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F97" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G97" s="6"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="119"/>
+      <c r="B98" s="120"/>
+      <c r="C98" s="120"/>
+      <c r="D98" s="120"/>
+      <c r="E98" s="120"/>
+      <c r="F98" s="121"/>
+    </row>
+    <row r="99" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="B99" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D99" s="22"/>
+      <c r="E99" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F99" s="22"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="98"/>
+      <c r="B100" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C100" s="22"/>
+      <c r="D100" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F100" s="22"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="98"/>
+      <c r="B101" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C101" s="22"/>
+      <c r="D101" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E101" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F101" s="22"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="98"/>
+      <c r="B102" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C102" s="22"/>
+      <c r="D102" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="F102" s="22"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="98"/>
+      <c r="B103" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D103" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="E103" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F103" s="22"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="98"/>
+      <c r="B104" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C104" s="22"/>
+      <c r="D104" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="F104" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="98"/>
+      <c r="B105" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C105" s="22"/>
+      <c r="D105" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E105" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F105" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="98"/>
+      <c r="B106" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C106" s="22"/>
+      <c r="D106" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F106" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="101"/>
+      <c r="B107" s="102"/>
+      <c r="C107" s="102"/>
+      <c r="D107" s="102"/>
+      <c r="E107" s="102"/>
+      <c r="F107" s="103"/>
+    </row>
+    <row r="108" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="133" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="85" t="s">
-        <v>227</v>
-      </c>
-      <c r="B15" s="86"/>
-      <c r="C15" s="56" t="s">
-        <v>235</v>
-      </c>
-      <c r="D15" s="56" t="s">
-        <v>168</v>
-      </c>
-      <c r="E15" s="67"/>
-    </row>
-    <row r="16" spans="1:6" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="118" t="s">
-        <v>238</v>
-      </c>
-      <c r="B16" s="118"/>
-      <c r="C16" s="62" t="s">
-        <v>232</v>
-      </c>
-      <c r="D16" s="57" t="s">
-        <v>226</v>
-      </c>
-      <c r="E16" s="68"/>
-    </row>
-    <row r="17" spans="1:5" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="118"/>
-      <c r="B17" s="118"/>
-      <c r="C17" s="61" t="s">
-        <v>234</v>
-      </c>
-      <c r="D17" s="58" t="s">
-        <v>224</v>
-      </c>
-      <c r="E17" s="68"/>
-    </row>
-    <row r="18" spans="1:5" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="118"/>
-      <c r="B18" s="118"/>
-      <c r="C18" s="63" t="s">
-        <v>233</v>
-      </c>
-      <c r="D18" s="64" t="s">
-        <v>230</v>
-      </c>
-      <c r="E18" s="68"/>
-    </row>
-    <row r="19" spans="1:5" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="118"/>
-      <c r="B19" s="118"/>
-      <c r="C19" s="65" t="s">
-        <v>236</v>
-      </c>
-      <c r="D19" s="59" t="s">
-        <v>231</v>
-      </c>
-      <c r="E19" s="68"/>
-    </row>
-    <row r="20" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="118"/>
-      <c r="B20" s="118"/>
-      <c r="C20" s="66" t="s">
-        <v>237</v>
-      </c>
-      <c r="D20" s="60" t="s">
-        <v>225</v>
-      </c>
-      <c r="E20" s="68"/>
-    </row>
-    <row r="21" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="68"/>
-    </row>
-    <row r="22" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="119" t="s">
-        <v>162</v>
-      </c>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="119" t="s">
-        <v>179</v>
-      </c>
-      <c r="E22" s="119"/>
-    </row>
-    <row r="23" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="E23" s="41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="D24" s="121" t="s">
-        <v>166</v>
-      </c>
-      <c r="E24" s="121" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="4">
+      <c r="C108" s="26"/>
+      <c r="D108" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E108" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="F108" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="107"/>
+      <c r="B109" s="108"/>
+      <c r="C109" s="108"/>
+      <c r="D109" s="108"/>
+      <c r="E109" s="108"/>
+      <c r="F109" s="109"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="121"/>
-      <c r="E25" s="121"/>
-    </row>
-    <row r="26" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="5">
-        <v>45575.507002314815</v>
-      </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="121"/>
-      <c r="E26" s="121"/>
-    </row>
-    <row r="27" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="121"/>
-      <c r="E27" s="121"/>
-    </row>
-    <row r="28" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="121"/>
-      <c r="E28" s="121"/>
-    </row>
-    <row r="29" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-    </row>
-    <row r="30" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="4">
-        <v>11000</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="D30" s="121"/>
-      <c r="E30" s="121"/>
-    </row>
-    <row r="31" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" s="4">
-        <v>100</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="121"/>
-      <c r="E31" s="121"/>
-    </row>
-    <row r="32" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="4">
-        <v>110</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="121"/>
-      <c r="E32" s="121"/>
-    </row>
-    <row r="33" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33" s="4">
+      <c r="B110" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="121"/>
-      <c r="E33" s="121"/>
-    </row>
-    <row r="34" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="122" t="s">
-        <v>131</v>
-      </c>
-      <c r="B34" s="124" t="s">
-        <v>210</v>
-      </c>
-      <c r="C34" s="125"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="121"/>
-    </row>
-    <row r="35" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="123"/>
-      <c r="B35" s="126" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" s="127"/>
-      <c r="D35" s="121"/>
-      <c r="E35" s="121"/>
-    </row>
-    <row r="36" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C36" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D36" s="121"/>
-      <c r="E36" s="121"/>
-    </row>
-    <row r="37" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C37" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="D37" s="121"/>
-      <c r="E37" s="121"/>
-    </row>
-    <row r="38" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B38" s="4">
-        <v>6</v>
-      </c>
-      <c r="C38" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="D38" s="121"/>
-      <c r="E38" s="121"/>
-    </row>
-    <row r="39" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B39" s="4">
-        <v>10</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39" s="121"/>
-      <c r="E39" s="121"/>
-    </row>
-    <row r="40" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B40" s="128" t="s">
-        <v>229</v>
-      </c>
-      <c r="C40" s="128"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-    </row>
-    <row r="41" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="70"/>
-      <c r="B41" s="70"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="68"/>
-    </row>
-    <row r="42" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="84" t="s">
-        <v>161</v>
-      </c>
-      <c r="B42" s="84"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="84"/>
-      <c r="E42" s="84"/>
-      <c r="F42" s="84"/>
-    </row>
-    <row r="43" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="87" t="s">
-        <v>191</v>
-      </c>
-      <c r="B44" s="88"/>
-      <c r="C44" s="88"/>
-      <c r="D44" s="88"/>
-      <c r="E44" s="88"/>
-    </row>
-    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="E45" s="33" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="B46" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="C46" s="94"/>
-      <c r="D46" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="E46" s="91" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="B47" s="35" t="s">
-        <v>200</v>
-      </c>
-      <c r="C47" s="96"/>
-      <c r="D47" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E47" s="92"/>
-    </row>
-    <row r="48" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="C48" s="96"/>
-      <c r="D48" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="E48" s="92"/>
-    </row>
-    <row r="49" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="B49" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="C49" s="96"/>
-      <c r="D49" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="E49" s="92"/>
-    </row>
-    <row r="50" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="52" t="s">
-        <v>190</v>
-      </c>
-      <c r="B50" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="C50" s="96"/>
-      <c r="D50" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="E50" s="92"/>
-    </row>
-    <row r="51" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="52" t="s">
-        <v>207</v>
-      </c>
-      <c r="B51" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="C51" s="95"/>
-      <c r="D51" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="E51" s="93"/>
-    </row>
-    <row r="52" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="B52" s="94"/>
-      <c r="C52" s="53" t="s">
-        <v>212</v>
-      </c>
-      <c r="D52" s="50" t="s">
-        <v>213</v>
-      </c>
-      <c r="E52" s="89" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="B53" s="95"/>
-      <c r="C53" s="54" t="s">
-        <v>204</v>
-      </c>
-      <c r="D53" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="E53" s="90"/>
-    </row>
-    <row r="55" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="88" t="s">
-        <v>178</v>
-      </c>
-      <c r="B55" s="88"/>
-      <c r="C55" s="88"/>
-      <c r="D55" s="88"/>
-      <c r="E55" s="88"/>
-      <c r="F55" s="88"/>
-    </row>
-    <row r="56" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A56" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B56" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="C56" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="D56" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="F56" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="G56" s="6"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="97" t="s">
-        <v>128</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="G57" s="6"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-    </row>
-    <row r="58" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="97"/>
-      <c r="B58" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="F58" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G58" s="6"/>
-    </row>
-    <row r="59" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="97"/>
-      <c r="B59" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D59" s="9"/>
-      <c r="E59" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F59" s="12"/>
-      <c r="G59" s="6"/>
-    </row>
-    <row r="60" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="97"/>
-      <c r="B60" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="G60" s="6"/>
-    </row>
-    <row r="61" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="97"/>
-      <c r="B61" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="G61" s="6"/>
-    </row>
-    <row r="62" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="97"/>
-      <c r="B62" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F62" s="9"/>
-      <c r="G62" s="6"/>
-    </row>
-    <row r="63" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="97"/>
-      <c r="B63" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F63" s="9"/>
-      <c r="G63" s="6"/>
-    </row>
-    <row r="64" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="97"/>
-      <c r="B64" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F64" s="9"/>
-      <c r="G64" s="6"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="97"/>
-      <c r="B65" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G65" s="6"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="97"/>
-      <c r="B66" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G66" s="6"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="97"/>
-      <c r="B67" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G67" s="6"/>
-    </row>
-    <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="78"/>
-      <c r="B68" s="79"/>
-      <c r="C68" s="79"/>
-      <c r="D68" s="79"/>
-      <c r="E68" s="79"/>
-      <c r="F68" s="80"/>
-      <c r="G68" s="6"/>
-    </row>
-    <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="98" t="s">
-        <v>127</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G69" s="6"/>
-    </row>
-    <row r="70" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="98"/>
-      <c r="B70" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G70" s="6"/>
-    </row>
-    <row r="71" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="98"/>
-      <c r="B71" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="6"/>
-    </row>
-    <row r="72" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="98"/>
-      <c r="B72" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C72" s="7"/>
-      <c r="D72" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G72" s="6"/>
-    </row>
-    <row r="73" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="78"/>
-      <c r="B73" s="79"/>
-      <c r="C73" s="79"/>
-      <c r="D73" s="79"/>
-      <c r="E73" s="79"/>
-      <c r="F73" s="80"/>
-      <c r="G73" s="6"/>
-    </row>
-    <row r="74" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A74" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74" s="14"/>
-      <c r="D74" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E74" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="F74" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="G74" s="6"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="81"/>
-      <c r="B75" s="82"/>
-      <c r="C75" s="82"/>
-      <c r="D75" s="82"/>
-      <c r="E75" s="82"/>
-      <c r="F75" s="83"/>
-    </row>
-    <row r="76" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="109" t="s">
-        <v>32</v>
-      </c>
-      <c r="B76" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C76" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D76" s="22"/>
-      <c r="E76" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="F76" s="22"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="109"/>
-      <c r="B77" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C77" s="22"/>
-      <c r="D77" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E77" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="F77" s="22"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="109"/>
-      <c r="B78" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C78" s="22"/>
-      <c r="D78" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F78" s="22"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="109"/>
-      <c r="B79" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="C79" s="22"/>
-      <c r="D79" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E79" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="F79" s="22"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="109"/>
-      <c r="B80" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C80" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D80" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="E80" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="F80" s="22"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="109"/>
-      <c r="B81" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E81" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="F81" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="109"/>
-      <c r="B82" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E82" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F82" s="22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="109"/>
-      <c r="B83" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C83" s="22"/>
-      <c r="D83" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E83" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F83" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="112"/>
-      <c r="B84" s="113"/>
-      <c r="C84" s="113"/>
-      <c r="D84" s="113"/>
-      <c r="E84" s="113"/>
-      <c r="F84" s="114"/>
-    </row>
-    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B85" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" s="26"/>
-      <c r="D85" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="E85" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="F85" s="28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="101"/>
-      <c r="B86" s="102"/>
-      <c r="C86" s="102"/>
-      <c r="D86" s="102"/>
-      <c r="E86" s="102"/>
-      <c r="F86" s="103"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="110" t="s">
-        <v>1</v>
-      </c>
-      <c r="B87" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C87" s="29" t="s">
+      <c r="C110" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="D87" s="29"/>
-      <c r="E87" s="30" t="s">
+      <c r="D110" s="29"/>
+      <c r="E110" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="F87" s="29" t="s">
+      <c r="F110" s="29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="110"/>
-      <c r="B88" s="29" t="s">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="99"/>
+      <c r="B111" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C88" s="29"/>
-      <c r="D88" s="29" t="s">
+      <c r="C111" s="29"/>
+      <c r="D111" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="30" t="s">
+      <c r="E111" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F88" s="29"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="110"/>
-      <c r="B89" s="29" t="s">
+      <c r="F111" s="29"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="99"/>
+      <c r="B112" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C89" s="29" t="s">
+      <c r="C112" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D89" s="29"/>
-      <c r="E89" s="30" t="s">
+      <c r="D112" s="29"/>
+      <c r="E112" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F89" s="29" t="s">
+      <c r="F112" s="29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="110"/>
-      <c r="B90" s="29" t="s">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="99"/>
+      <c r="B113" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C90" s="29"/>
-      <c r="D90" s="31" t="s">
+      <c r="C113" s="29"/>
+      <c r="D113" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E90" s="30" t="s">
+      <c r="E113" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F90" s="29"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="104"/>
-      <c r="B91" s="105"/>
-      <c r="C91" s="105"/>
-      <c r="D91" s="105"/>
-      <c r="E91" s="105"/>
-      <c r="F91" s="106"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="107" t="s">
+      <c r="F113" s="29"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="110"/>
+      <c r="B114" s="111"/>
+      <c r="C114" s="111"/>
+      <c r="D114" s="111"/>
+      <c r="E114" s="111"/>
+      <c r="F114" s="112"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="113" t="s">
         <v>217</v>
       </c>
-      <c r="B92" s="29" t="s">
+      <c r="B115" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="C92" s="29" t="s">
+      <c r="C115" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="D92" s="31"/>
-      <c r="E92" s="30" t="s">
+      <c r="D115" s="31"/>
+      <c r="E115" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="F92" s="29"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="108"/>
-      <c r="B93" s="29" t="s">
+      <c r="F115" s="29"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="114"/>
+      <c r="B116" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C93" s="29"/>
-      <c r="D93" s="31" t="s">
+      <c r="C116" s="29"/>
+      <c r="D116" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="E93" s="30" t="s">
+      <c r="E116" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="F93" s="29"/>
-    </row>
-    <row r="94" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="104"/>
-      <c r="B94" s="105"/>
-      <c r="C94" s="105"/>
-      <c r="D94" s="105"/>
-      <c r="E94" s="105"/>
-      <c r="F94" s="106"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="111" t="s">
+      <c r="F116" s="29"/>
+    </row>
+    <row r="117" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="110"/>
+      <c r="B117" s="111"/>
+      <c r="C117" s="111"/>
+      <c r="D117" s="111"/>
+      <c r="E117" s="111"/>
+      <c r="F117" s="112"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="B95" s="13" t="s">
+      <c r="B118" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C95" s="13" t="s">
+      <c r="C118" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D95" s="13"/>
-      <c r="E95" s="14" t="s">
+      <c r="D118" s="13"/>
+      <c r="E118" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F95" s="13" t="s">
+      <c r="F118" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="111"/>
-      <c r="B96" s="13" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="100"/>
+      <c r="B119" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C96" s="13"/>
-      <c r="D96" s="13" t="s">
+      <c r="C119" s="13"/>
+      <c r="D119" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E96" s="14" t="s">
+      <c r="E119" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F96" s="13" t="s">
+      <c r="F119" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="104"/>
-      <c r="B97" s="105"/>
-      <c r="C97" s="105"/>
-      <c r="D97" s="105"/>
-      <c r="E97" s="105"/>
-      <c r="F97" s="106"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="131" t="s">
+    <row r="120" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="110"/>
+      <c r="B120" s="111"/>
+      <c r="C120" s="111"/>
+      <c r="D120" s="111"/>
+      <c r="E120" s="111"/>
+      <c r="F120" s="112"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="B98" s="15" t="s">
+      <c r="B121" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C98" s="15" t="s">
+      <c r="C121" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D98" s="15"/>
-      <c r="E98" s="16" t="s">
+      <c r="D121" s="15"/>
+      <c r="E121" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F98" s="15" t="s">
+      <c r="F121" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="131"/>
-      <c r="B99" s="15" t="s">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="97"/>
+      <c r="B122" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C99" s="15"/>
-      <c r="D99" s="15" t="s">
+      <c r="C122" s="15"/>
+      <c r="D122" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E99" s="16" t="s">
+      <c r="E122" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F99" s="15" t="s">
+      <c r="F122" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="37"/>
-      <c r="E100" s="6"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="84" t="s">
+    <row r="123" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="37"/>
+      <c r="E123" s="6"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="B101" s="84"/>
-      <c r="C101" s="84"/>
-      <c r="D101" s="84"/>
-      <c r="E101" s="84"/>
-      <c r="F101" s="84"/>
-    </row>
-    <row r="103" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="115"/>
-      <c r="B103" s="116"/>
-      <c r="C103" s="116"/>
-      <c r="D103" s="115"/>
-      <c r="E103" s="115"/>
-    </row>
-    <row r="104" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="73"/>
-      <c r="B104" s="74"/>
-      <c r="C104" s="74"/>
-      <c r="D104" s="72"/>
-      <c r="E104" s="75"/>
-    </row>
-    <row r="105" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="2"/>
-      <c r="B105" s="55"/>
-      <c r="C105" s="55"/>
-      <c r="D105" s="100"/>
-      <c r="E105" s="100"/>
-    </row>
-    <row r="106" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="2"/>
-      <c r="B106" s="55"/>
-      <c r="C106" s="55"/>
-      <c r="D106" s="100"/>
-      <c r="E106" s="100"/>
-    </row>
-    <row r="107" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="2"/>
-      <c r="B107" s="76"/>
-      <c r="C107" s="55"/>
-      <c r="D107" s="100"/>
-      <c r="E107" s="100"/>
-    </row>
-    <row r="108" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="2"/>
-      <c r="B108" s="55"/>
-      <c r="C108" s="55"/>
-      <c r="D108" s="100"/>
-      <c r="E108" s="100"/>
-    </row>
-    <row r="109" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="2"/>
-      <c r="B109" s="55"/>
-      <c r="C109" s="55"/>
-      <c r="D109" s="100"/>
-      <c r="E109" s="100"/>
-    </row>
-    <row r="110" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="2"/>
-      <c r="B110" s="55"/>
-      <c r="C110" s="55"/>
-      <c r="D110" s="100"/>
-      <c r="E110" s="100"/>
-    </row>
-    <row r="111" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="2"/>
-      <c r="B111" s="55"/>
-      <c r="C111" s="55"/>
-      <c r="D111" s="100"/>
-      <c r="E111" s="100"/>
-    </row>
-    <row r="112" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="2"/>
-      <c r="B112" s="55"/>
-      <c r="C112" s="55"/>
-      <c r="D112" s="100"/>
-      <c r="E112" s="100"/>
-    </row>
-    <row r="113" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="2"/>
-      <c r="B113" s="55"/>
-      <c r="C113" s="55"/>
-      <c r="D113" s="100"/>
-      <c r="E113" s="100"/>
-    </row>
-    <row r="114" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="2"/>
-      <c r="B114" s="55"/>
-      <c r="C114" s="55"/>
-      <c r="D114" s="100"/>
-      <c r="E114" s="100"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="99"/>
-      <c r="B115" s="130"/>
-      <c r="C115" s="130"/>
-      <c r="D115" s="100"/>
-      <c r="E115" s="100"/>
-    </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="99"/>
-      <c r="B116" s="129"/>
-      <c r="C116" s="129"/>
-      <c r="D116" s="100"/>
-      <c r="E116" s="100"/>
-    </row>
-    <row r="117" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="2"/>
-      <c r="B117" s="55"/>
-      <c r="C117" s="55"/>
-      <c r="D117" s="100"/>
-      <c r="E117" s="100"/>
-    </row>
-    <row r="118" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="2"/>
-      <c r="B118" s="55"/>
-      <c r="C118" s="55"/>
-      <c r="D118" s="100"/>
-      <c r="E118" s="100"/>
-    </row>
-    <row r="119" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="2"/>
-      <c r="B119" s="55"/>
-      <c r="C119" s="55"/>
-      <c r="D119" s="100"/>
-      <c r="E119" s="100"/>
-    </row>
-    <row r="120" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="2"/>
-      <c r="B120" s="55"/>
-      <c r="C120" s="55"/>
-      <c r="D120" s="100"/>
-      <c r="E120" s="100"/>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="2"/>
-      <c r="B121" s="117"/>
-      <c r="C121" s="117"/>
-      <c r="D121" s="38"/>
-      <c r="E121" s="38"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D122" s="38"/>
-      <c r="E122" s="38"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D123" s="38"/>
-      <c r="E123" s="38"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D124" s="38"/>
-      <c r="E124" s="38"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D125" s="38"/>
-      <c r="E125" s="38"/>
+      <c r="B124" s="96"/>
+      <c r="C124" s="96"/>
+      <c r="D124" s="96"/>
+      <c r="E124" s="96"/>
+      <c r="F124" s="96"/>
+    </row>
+    <row r="126" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="95"/>
+      <c r="B126" s="104"/>
+      <c r="C126" s="104"/>
+      <c r="D126" s="95"/>
+      <c r="E126" s="95"/>
+    </row>
+    <row r="127" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="73"/>
+      <c r="B127" s="74"/>
+      <c r="C127" s="74"/>
+      <c r="D127" s="72"/>
+      <c r="E127" s="75"/>
+    </row>
+    <row r="128" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2"/>
+      <c r="B128" s="55"/>
+      <c r="C128" s="55"/>
+      <c r="D128" s="106"/>
+      <c r="E128" s="106"/>
+    </row>
+    <row r="129" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2"/>
+      <c r="B129" s="55"/>
+      <c r="C129" s="55"/>
+      <c r="D129" s="106"/>
+      <c r="E129" s="106"/>
+    </row>
+    <row r="130" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2"/>
+      <c r="B130" s="76"/>
+      <c r="C130" s="55"/>
+      <c r="D130" s="106"/>
+      <c r="E130" s="106"/>
+    </row>
+    <row r="131" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2"/>
+      <c r="B131" s="55"/>
+      <c r="C131" s="55"/>
+      <c r="D131" s="106"/>
+      <c r="E131" s="106"/>
+    </row>
+    <row r="132" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
+      <c r="B132" s="55"/>
+      <c r="C132" s="55"/>
+      <c r="D132" s="106"/>
+      <c r="E132" s="106"/>
+    </row>
+    <row r="133" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2"/>
+      <c r="B133" s="55"/>
+      <c r="C133" s="55"/>
+      <c r="D133" s="106"/>
+      <c r="E133" s="106"/>
+    </row>
+    <row r="134" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2"/>
+      <c r="B134" s="55"/>
+      <c r="C134" s="55"/>
+      <c r="D134" s="106"/>
+      <c r="E134" s="106"/>
+    </row>
+    <row r="135" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2"/>
+      <c r="B135" s="55"/>
+      <c r="C135" s="55"/>
+      <c r="D135" s="106"/>
+      <c r="E135" s="106"/>
+    </row>
+    <row r="136" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2"/>
+      <c r="B136" s="55"/>
+      <c r="C136" s="55"/>
+      <c r="D136" s="106"/>
+      <c r="E136" s="106"/>
+    </row>
+    <row r="137" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2"/>
+      <c r="B137" s="55"/>
+      <c r="C137" s="55"/>
+      <c r="D137" s="106"/>
+      <c r="E137" s="106"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="105"/>
+      <c r="B138" s="93"/>
+      <c r="C138" s="93"/>
+      <c r="D138" s="106"/>
+      <c r="E138" s="106"/>
+    </row>
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="105"/>
+      <c r="B139" s="92"/>
+      <c r="C139" s="92"/>
+      <c r="D139" s="106"/>
+      <c r="E139" s="106"/>
+    </row>
+    <row r="140" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2"/>
+      <c r="B140" s="55"/>
+      <c r="C140" s="55"/>
+      <c r="D140" s="106"/>
+      <c r="E140" s="106"/>
+    </row>
+    <row r="141" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+      <c r="B141" s="55"/>
+      <c r="C141" s="55"/>
+      <c r="D141" s="106"/>
+      <c r="E141" s="106"/>
+    </row>
+    <row r="142" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2"/>
+      <c r="B142" s="55"/>
+      <c r="C142" s="55"/>
+      <c r="D142" s="106"/>
+      <c r="E142" s="106"/>
+    </row>
+    <row r="143" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2"/>
+      <c r="B143" s="55"/>
+      <c r="C143" s="55"/>
+      <c r="D143" s="106"/>
+      <c r="E143" s="106"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+      <c r="B144" s="80"/>
+      <c r="C144" s="80"/>
+      <c r="D144" s="38"/>
+      <c r="E144" s="38"/>
+    </row>
+    <row r="145" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D145" s="38"/>
+      <c r="E145" s="38"/>
+    </row>
+    <row r="146" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D146" s="38"/>
+      <c r="E146" s="38"/>
+    </row>
+    <row r="147" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D147" s="38"/>
+      <c r="E147" s="38"/>
+    </row>
+    <row r="148" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D148" s="38"/>
+      <c r="E148" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="A16:B20"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D24:D39"/>
-    <mergeCell ref="E24:E39"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="A101:F101"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A76:A83"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A84:F84"/>
-    <mergeCell ref="A103:C103"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A96:F96"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="E69:E74"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="A80:A90"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="D128:D143"/>
+    <mergeCell ref="E128:E143"/>
+    <mergeCell ref="A109:F109"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="A120:F120"/>
+    <mergeCell ref="A114:F114"/>
     <mergeCell ref="A115:A116"/>
-    <mergeCell ref="D105:D120"/>
-    <mergeCell ref="E105:E120"/>
-    <mergeCell ref="A86:F86"/>
-    <mergeCell ref="A94:F94"/>
-    <mergeCell ref="A97:F97"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="E46:E51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C46:C51"/>
-    <mergeCell ref="A57:A67"/>
-    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A99:A106"/>
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A107:F107"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="A39:B43"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D47:D62"/>
+    <mergeCell ref="E47:E62"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="A124:F124"/>
+    <mergeCell ref="A121:A122"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
unrecognitionCount value range reduce by 1
</commit_message>
<xml_diff>
--- a/THT-Face/doc/CMD list of Face attendence .xlsx
+++ b/THT-Face/doc/CMD list of Face attendence .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\THT-Face\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E6FBD4-FD17-4449-9330-39276FC9E4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F29602-B05F-46C2-A319-BDF19DB8FB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28920" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -2227,6 +2227,138 @@
     <xf numFmtId="0" fontId="15" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2269,140 +2401,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2749,8 +2749,8 @@
   </sheetPr>
   <dimension ref="A1:N148"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,28 +2772,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="84" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="115"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
     </row>
     <row r="4" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="92" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="123"/>
+      <c r="B4" s="93"/>
     </row>
     <row r="5" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
@@ -2909,12 +2909,12 @@
       </c>
     </row>
     <row r="20" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="135"/>
-      <c r="B20" s="136"/>
+      <c r="A20" s="80"/>
+      <c r="B20" s="81"/>
     </row>
     <row r="21" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="135"/>
-      <c r="B21" s="136"/>
+      <c r="A21" s="80"/>
+      <c r="B21" s="81"/>
     </row>
     <row r="22" spans="1:2" s="42" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="79" t="s">
@@ -2925,118 +2925,118 @@
       </c>
     </row>
     <row r="23" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="137">
+      <c r="A23" s="82">
         <v>1</v>
       </c>
-      <c r="B23" s="138" t="s">
+      <c r="B23" s="83" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="137">
+      <c r="A24" s="82">
         <v>2</v>
       </c>
-      <c r="B24" s="138" t="s">
+      <c r="B24" s="83" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="137">
+      <c r="A25" s="82">
         <v>3</v>
       </c>
-      <c r="B25" s="138" t="s">
+      <c r="B25" s="83" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="137">
+      <c r="A26" s="82">
         <v>4</v>
       </c>
-      <c r="B26" s="138" t="s">
+      <c r="B26" s="83" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="137">
+      <c r="A27" s="82">
         <v>5</v>
       </c>
-      <c r="B27" s="138" t="s">
+      <c r="B27" s="83" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="137">
+      <c r="A28" s="82">
         <v>6</v>
       </c>
-      <c r="B28" s="138" t="s">
+      <c r="B28" s="83" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="137">
+      <c r="A29" s="82">
         <v>7</v>
       </c>
-      <c r="B29" s="138" t="s">
+      <c r="B29" s="83" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="137">
+      <c r="A30" s="82">
         <v>8</v>
       </c>
-      <c r="B30" s="138" t="s">
+      <c r="B30" s="83" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="137">
+      <c r="A31" s="82">
         <v>9</v>
       </c>
-      <c r="B31" s="138" t="s">
+      <c r="B31" s="83" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="137">
+      <c r="A32" s="82">
         <v>10</v>
       </c>
-      <c r="B32" s="138" t="s">
+      <c r="B32" s="83" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="137">
+      <c r="A33" s="82">
         <v>11</v>
       </c>
-      <c r="B33" s="138" t="s">
+      <c r="B33" s="83" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="137">
+      <c r="A34" s="82">
         <v>12</v>
       </c>
-      <c r="B34" s="138" t="s">
+      <c r="B34" s="83" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="135"/>
-      <c r="B35" s="136"/>
+      <c r="A35" s="80"/>
+      <c r="B35" s="81"/>
     </row>
     <row r="36" spans="1:5" s="42" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="135"/>
-      <c r="B36" s="136"/>
+      <c r="A36" s="80"/>
+      <c r="B36" s="81"/>
     </row>
     <row r="37" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:5" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="122" t="s">
+      <c r="A38" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="B38" s="123"/>
+      <c r="B38" s="93"/>
       <c r="C38" s="56" t="s">
         <v>235</v>
       </c>
@@ -3046,10 +3046,10 @@
       <c r="E38" s="67"/>
     </row>
     <row r="39" spans="1:5" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="81" t="s">
+      <c r="A39" s="125" t="s">
         <v>238</v>
       </c>
-      <c r="B39" s="81"/>
+      <c r="B39" s="125"/>
       <c r="C39" s="62" t="s">
         <v>232</v>
       </c>
@@ -3059,8 +3059,8 @@
       <c r="E39" s="68"/>
     </row>
     <row r="40" spans="1:5" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="81"/>
-      <c r="B40" s="81"/>
+      <c r="A40" s="125"/>
+      <c r="B40" s="125"/>
       <c r="C40" s="61" t="s">
         <v>234</v>
       </c>
@@ -3070,8 +3070,8 @@
       <c r="E40" s="68"/>
     </row>
     <row r="41" spans="1:5" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="81"/>
-      <c r="B41" s="81"/>
+      <c r="A41" s="125"/>
+      <c r="B41" s="125"/>
       <c r="C41" s="63" t="s">
         <v>233</v>
       </c>
@@ -3081,8 +3081,8 @@
       <c r="E41" s="68"/>
     </row>
     <row r="42" spans="1:5" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="81"/>
-      <c r="B42" s="81"/>
+      <c r="A42" s="125"/>
+      <c r="B42" s="125"/>
       <c r="C42" s="65" t="s">
         <v>236</v>
       </c>
@@ -3092,8 +3092,8 @@
       <c r="E42" s="68"/>
     </row>
     <row r="43" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="81"/>
-      <c r="B43" s="81"/>
+      <c r="A43" s="125"/>
+      <c r="B43" s="125"/>
       <c r="C43" s="66" t="s">
         <v>237</v>
       </c>
@@ -3110,15 +3110,15 @@
       <c r="E44" s="68"/>
     </row>
     <row r="45" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="82" t="s">
+      <c r="A45" s="126" t="s">
         <v>162</v>
       </c>
-      <c r="B45" s="83"/>
-      <c r="C45" s="83"/>
-      <c r="D45" s="82" t="s">
+      <c r="B45" s="127"/>
+      <c r="C45" s="127"/>
+      <c r="D45" s="126" t="s">
         <v>179</v>
       </c>
-      <c r="E45" s="82"/>
+      <c r="E45" s="126"/>
     </row>
     <row r="46" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="47" t="s">
@@ -3147,10 +3147,10 @@
       <c r="C47" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="D47" s="84" t="s">
+      <c r="D47" s="128" t="s">
         <v>166</v>
       </c>
-      <c r="E47" s="84" t="s">
+      <c r="E47" s="128" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3164,8 +3164,8 @@
       <c r="C48" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="D48" s="84"/>
-      <c r="E48" s="84"/>
+      <c r="D48" s="128"/>
+      <c r="E48" s="128"/>
     </row>
     <row r="49" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
@@ -3175,8 +3175,8 @@
         <v>45575.507002314815</v>
       </c>
       <c r="C49" s="39"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="84"/>
+      <c r="D49" s="128"/>
+      <c r="E49" s="128"/>
     </row>
     <row r="50" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
@@ -3188,8 +3188,8 @@
       <c r="C50" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="D50" s="84"/>
-      <c r="E50" s="84"/>
+      <c r="D50" s="128"/>
+      <c r="E50" s="128"/>
     </row>
     <row r="51" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
@@ -3201,8 +3201,8 @@
       <c r="C51" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="84"/>
-      <c r="E51" s="84"/>
+      <c r="D51" s="128"/>
+      <c r="E51" s="128"/>
     </row>
     <row r="52" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
@@ -3212,8 +3212,8 @@
       <c r="C52" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
+      <c r="D52" s="128"/>
+      <c r="E52" s="128"/>
     </row>
     <row r="53" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
@@ -3225,8 +3225,8 @@
       <c r="C53" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="D53" s="84"/>
-      <c r="E53" s="84"/>
+      <c r="D53" s="128"/>
+      <c r="E53" s="128"/>
     </row>
     <row r="54" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
@@ -3238,8 +3238,8 @@
       <c r="C54" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="84"/>
-      <c r="E54" s="84"/>
+      <c r="D54" s="128"/>
+      <c r="E54" s="128"/>
     </row>
     <row r="55" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
@@ -3251,8 +3251,8 @@
       <c r="C55" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="84"/>
-      <c r="E55" s="84"/>
+      <c r="D55" s="128"/>
+      <c r="E55" s="128"/>
     </row>
     <row r="56" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
@@ -3264,28 +3264,28 @@
       <c r="C56" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="84"/>
-      <c r="E56" s="84"/>
+      <c r="D56" s="128"/>
+      <c r="E56" s="128"/>
     </row>
     <row r="57" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="85" t="s">
+      <c r="A57" s="129" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="87" t="s">
+      <c r="B57" s="131" t="s">
         <v>210</v>
       </c>
-      <c r="C57" s="88"/>
-      <c r="D57" s="84"/>
-      <c r="E57" s="84"/>
+      <c r="C57" s="132"/>
+      <c r="D57" s="128"/>
+      <c r="E57" s="128"/>
     </row>
     <row r="58" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="86"/>
-      <c r="B58" s="89" t="s">
+      <c r="A58" s="130"/>
+      <c r="B58" s="133" t="s">
         <v>134</v>
       </c>
-      <c r="C58" s="90"/>
-      <c r="D58" s="84"/>
-      <c r="E58" s="84"/>
+      <c r="C58" s="134"/>
+      <c r="D58" s="128"/>
+      <c r="E58" s="128"/>
     </row>
     <row r="59" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
@@ -3297,8 +3297,8 @@
       <c r="C59" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="D59" s="84"/>
-      <c r="E59" s="84"/>
+      <c r="D59" s="128"/>
+      <c r="E59" s="128"/>
     </row>
     <row r="60" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
@@ -3310,8 +3310,8 @@
       <c r="C60" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="D60" s="84"/>
-      <c r="E60" s="84"/>
+      <c r="D60" s="128"/>
+      <c r="E60" s="128"/>
     </row>
     <row r="61" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
@@ -3323,8 +3323,8 @@
       <c r="C61" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="D61" s="84"/>
-      <c r="E61" s="84"/>
+      <c r="D61" s="128"/>
+      <c r="E61" s="128"/>
     </row>
     <row r="62" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -3336,17 +3336,17 @@
       <c r="C62" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="D62" s="84"/>
-      <c r="E62" s="84"/>
+      <c r="D62" s="128"/>
+      <c r="E62" s="128"/>
     </row>
     <row r="63" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B63" s="91" t="s">
+      <c r="B63" s="135" t="s">
         <v>229</v>
       </c>
-      <c r="C63" s="91"/>
+      <c r="C63" s="135"/>
       <c r="D63" s="38"/>
       <c r="E63" s="38"/>
     </row>
@@ -3358,27 +3358,27 @@
       <c r="E64" s="68"/>
     </row>
     <row r="65" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="96" t="s">
+      <c r="A65" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="96"/>
-      <c r="C65" s="96"/>
-      <c r="D65" s="96"/>
-      <c r="E65" s="96"/>
-      <c r="F65" s="96"/>
+      <c r="B65" s="91"/>
+      <c r="C65" s="91"/>
+      <c r="D65" s="91"/>
+      <c r="E65" s="91"/>
+      <c r="F65" s="91"/>
     </row>
     <row r="66" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
     </row>
     <row r="67" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="124" t="s">
+      <c r="A67" s="94" t="s">
         <v>191</v>
       </c>
-      <c r="B67" s="94"/>
-      <c r="C67" s="94"/>
-      <c r="D67" s="94"/>
-      <c r="E67" s="94"/>
+      <c r="B67" s="95"/>
+      <c r="C67" s="95"/>
+      <c r="D67" s="95"/>
+      <c r="E67" s="95"/>
     </row>
     <row r="68" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="51" t="s">
@@ -3404,11 +3404,11 @@
       <c r="B69" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="C69" s="130"/>
+      <c r="C69" s="101"/>
       <c r="D69" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="E69" s="127" t="s">
+      <c r="E69" s="98" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3419,11 +3419,11 @@
       <c r="B70" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="C70" s="132"/>
+      <c r="C70" s="103"/>
       <c r="D70" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E70" s="128"/>
+      <c r="E70" s="99"/>
     </row>
     <row r="71" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="52" t="s">
@@ -3432,11 +3432,11 @@
       <c r="B71" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="C71" s="132"/>
+      <c r="C71" s="103"/>
       <c r="D71" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="E71" s="128"/>
+      <c r="E71" s="99"/>
     </row>
     <row r="72" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="52" t="s">
@@ -3445,11 +3445,11 @@
       <c r="B72" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="C72" s="132"/>
+      <c r="C72" s="103"/>
       <c r="D72" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="E72" s="128"/>
+      <c r="E72" s="99"/>
     </row>
     <row r="73" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="52" t="s">
@@ -3458,11 +3458,11 @@
       <c r="B73" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="C73" s="132"/>
+      <c r="C73" s="103"/>
       <c r="D73" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="E73" s="128"/>
+      <c r="E73" s="99"/>
     </row>
     <row r="74" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="52" t="s">
@@ -3471,24 +3471,24 @@
       <c r="B74" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="C74" s="131"/>
+      <c r="C74" s="102"/>
       <c r="D74" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="E74" s="129"/>
+      <c r="E74" s="100"/>
     </row>
     <row r="75" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="B75" s="130"/>
+      <c r="B75" s="101"/>
       <c r="C75" s="53" t="s">
         <v>212</v>
       </c>
       <c r="D75" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="E75" s="125" t="s">
+      <c r="E75" s="96" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3496,24 +3496,24 @@
       <c r="A76" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="B76" s="131"/>
+      <c r="B76" s="102"/>
       <c r="C76" s="54" t="s">
         <v>204</v>
       </c>
       <c r="D76" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E76" s="126"/>
+      <c r="E76" s="97"/>
     </row>
     <row r="78" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="94" t="s">
+      <c r="A78" s="95" t="s">
         <v>178</v>
       </c>
-      <c r="B78" s="94"/>
-      <c r="C78" s="94"/>
-      <c r="D78" s="94"/>
-      <c r="E78" s="94"/>
-      <c r="F78" s="94"/>
+      <c r="B78" s="95"/>
+      <c r="C78" s="95"/>
+      <c r="D78" s="95"/>
+      <c r="E78" s="95"/>
+      <c r="F78" s="95"/>
     </row>
     <row r="79" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A79" s="46" t="s">
@@ -3539,7 +3539,7 @@
       <c r="N79" s="1"/>
     </row>
     <row r="80" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="133" t="s">
+      <c r="A80" s="104" t="s">
         <v>128</v>
       </c>
       <c r="B80" s="9" t="s">
@@ -3560,7 +3560,7 @@
       <c r="N80" s="1"/>
     </row>
     <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="133"/>
+      <c r="A81" s="104"/>
       <c r="B81" s="9" t="s">
         <v>6</v>
       </c>
@@ -3577,7 +3577,7 @@
       <c r="G81" s="6"/>
     </row>
     <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="133"/>
+      <c r="A82" s="104"/>
       <c r="B82" s="9" t="s">
         <v>107</v>
       </c>
@@ -3592,7 +3592,7 @@
       <c r="G82" s="6"/>
     </row>
     <row r="83" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="133"/>
+      <c r="A83" s="104"/>
       <c r="B83" s="10" t="s">
         <v>30</v>
       </c>
@@ -3609,7 +3609,7 @@
       <c r="G83" s="6"/>
     </row>
     <row r="84" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="133"/>
+      <c r="A84" s="104"/>
       <c r="B84" s="10" t="s">
         <v>31</v>
       </c>
@@ -3626,7 +3626,7 @@
       <c r="G84" s="6"/>
     </row>
     <row r="85" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="133"/>
+      <c r="A85" s="104"/>
       <c r="B85" s="9" t="s">
         <v>98</v>
       </c>
@@ -3641,7 +3641,7 @@
       <c r="G85" s="6"/>
     </row>
     <row r="86" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="133"/>
+      <c r="A86" s="104"/>
       <c r="B86" s="9" t="s">
         <v>100</v>
       </c>
@@ -3656,7 +3656,7 @@
       <c r="G86" s="6"/>
     </row>
     <row r="87" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="133"/>
+      <c r="A87" s="104"/>
       <c r="B87" s="9" t="s">
         <v>103</v>
       </c>
@@ -3671,7 +3671,7 @@
       <c r="G87" s="6"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="133"/>
+      <c r="A88" s="104"/>
       <c r="B88" s="9" t="s">
         <v>7</v>
       </c>
@@ -3688,7 +3688,7 @@
       <c r="G88" s="6"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="133"/>
+      <c r="A89" s="104"/>
       <c r="B89" s="9" t="s">
         <v>25</v>
       </c>
@@ -3705,7 +3705,7 @@
       <c r="G89" s="6"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="133"/>
+      <c r="A90" s="104"/>
       <c r="B90" s="9" t="s">
         <v>8</v>
       </c>
@@ -3722,16 +3722,16 @@
       <c r="G90" s="6"/>
     </row>
     <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="116"/>
-      <c r="B91" s="117"/>
-      <c r="C91" s="117"/>
-      <c r="D91" s="117"/>
-      <c r="E91" s="117"/>
-      <c r="F91" s="118"/>
+      <c r="A91" s="85"/>
+      <c r="B91" s="86"/>
+      <c r="C91" s="86"/>
+      <c r="D91" s="86"/>
+      <c r="E91" s="86"/>
+      <c r="F91" s="87"/>
       <c r="G91" s="6"/>
     </row>
     <row r="92" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="134" t="s">
+      <c r="A92" s="105" t="s">
         <v>127</v>
       </c>
       <c r="B92" s="7" t="s">
@@ -3752,7 +3752,7 @@
       <c r="G92" s="6"/>
     </row>
     <row r="93" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="134"/>
+      <c r="A93" s="105"/>
       <c r="B93" s="7" t="s">
         <v>9</v>
       </c>
@@ -3769,7 +3769,7 @@
       <c r="G93" s="6"/>
     </row>
     <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="134"/>
+      <c r="A94" s="105"/>
       <c r="B94" s="7" t="s">
         <v>10</v>
       </c>
@@ -3786,7 +3786,7 @@
       <c r="G94" s="6"/>
     </row>
     <row r="95" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="134"/>
+      <c r="A95" s="105"/>
       <c r="B95" s="8" t="s">
         <v>20</v>
       </c>
@@ -3803,12 +3803,12 @@
       <c r="G95" s="6"/>
     </row>
     <row r="96" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="116"/>
-      <c r="B96" s="117"/>
-      <c r="C96" s="117"/>
-      <c r="D96" s="117"/>
-      <c r="E96" s="117"/>
-      <c r="F96" s="118"/>
+      <c r="A96" s="85"/>
+      <c r="B96" s="86"/>
+      <c r="C96" s="86"/>
+      <c r="D96" s="86"/>
+      <c r="E96" s="86"/>
+      <c r="F96" s="87"/>
       <c r="G96" s="6"/>
     </row>
     <row r="97" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -3831,15 +3831,15 @@
       <c r="G97" s="6"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="119"/>
-      <c r="B98" s="120"/>
-      <c r="C98" s="120"/>
-      <c r="D98" s="120"/>
-      <c r="E98" s="120"/>
-      <c r="F98" s="121"/>
+      <c r="A98" s="88"/>
+      <c r="B98" s="89"/>
+      <c r="C98" s="89"/>
+      <c r="D98" s="89"/>
+      <c r="E98" s="89"/>
+      <c r="F98" s="90"/>
     </row>
     <row r="99" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="98" t="s">
+      <c r="A99" s="116" t="s">
         <v>32</v>
       </c>
       <c r="B99" s="20" t="s">
@@ -3855,7 +3855,7 @@
       <c r="F99" s="22"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="98"/>
+      <c r="A100" s="116"/>
       <c r="B100" s="22" t="s">
         <v>36</v>
       </c>
@@ -3869,7 +3869,7 @@
       <c r="F100" s="22"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="98"/>
+      <c r="A101" s="116"/>
       <c r="B101" s="22" t="s">
         <v>109</v>
       </c>
@@ -3883,7 +3883,7 @@
       <c r="F101" s="22"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="98"/>
+      <c r="A102" s="116"/>
       <c r="B102" s="22" t="s">
         <v>111</v>
       </c>
@@ -3897,7 +3897,7 @@
       <c r="F102" s="22"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="98"/>
+      <c r="A103" s="116"/>
       <c r="B103" s="22" t="s">
         <v>34</v>
       </c>
@@ -3913,7 +3913,7 @@
       <c r="F103" s="22"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="98"/>
+      <c r="A104" s="116"/>
       <c r="B104" s="22" t="s">
         <v>35</v>
       </c>
@@ -3929,7 +3929,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="98"/>
+      <c r="A105" s="116"/>
       <c r="B105" s="22" t="s">
         <v>39</v>
       </c>
@@ -3945,7 +3945,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="98"/>
+      <c r="A106" s="116"/>
       <c r="B106" s="22" t="s">
         <v>51</v>
       </c>
@@ -3961,12 +3961,12 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="101"/>
-      <c r="B107" s="102"/>
-      <c r="C107" s="102"/>
-      <c r="D107" s="102"/>
-      <c r="E107" s="102"/>
-      <c r="F107" s="103"/>
+      <c r="A107" s="119"/>
+      <c r="B107" s="120"/>
+      <c r="C107" s="120"/>
+      <c r="D107" s="120"/>
+      <c r="E107" s="120"/>
+      <c r="F107" s="121"/>
     </row>
     <row r="108" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="25" t="s">
@@ -3987,15 +3987,15 @@
       </c>
     </row>
     <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="107"/>
-      <c r="B109" s="108"/>
-      <c r="C109" s="108"/>
-      <c r="D109" s="108"/>
-      <c r="E109" s="108"/>
-      <c r="F109" s="109"/>
+      <c r="A109" s="108"/>
+      <c r="B109" s="109"/>
+      <c r="C109" s="109"/>
+      <c r="D109" s="109"/>
+      <c r="E109" s="109"/>
+      <c r="F109" s="110"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="99" t="s">
+      <c r="A110" s="117" t="s">
         <v>1</v>
       </c>
       <c r="B110" s="29" t="s">
@@ -4013,7 +4013,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="99"/>
+      <c r="A111" s="117"/>
       <c r="B111" s="29" t="s">
         <v>92</v>
       </c>
@@ -4027,7 +4027,7 @@
       <c r="F111" s="29"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="99"/>
+      <c r="A112" s="117"/>
       <c r="B112" s="29" t="s">
         <v>53</v>
       </c>
@@ -4043,7 +4043,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="99"/>
+      <c r="A113" s="117"/>
       <c r="B113" s="29" t="s">
         <v>92</v>
       </c>
@@ -4057,15 +4057,15 @@
       <c r="F113" s="29"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="110"/>
-      <c r="B114" s="111"/>
-      <c r="C114" s="111"/>
-      <c r="D114" s="111"/>
-      <c r="E114" s="111"/>
-      <c r="F114" s="112"/>
+      <c r="A114" s="111"/>
+      <c r="B114" s="112"/>
+      <c r="C114" s="112"/>
+      <c r="D114" s="112"/>
+      <c r="E114" s="112"/>
+      <c r="F114" s="113"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="113" t="s">
+      <c r="A115" s="114" t="s">
         <v>217</v>
       </c>
       <c r="B115" s="29" t="s">
@@ -4081,7 +4081,7 @@
       <c r="F115" s="29"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="114"/>
+      <c r="A116" s="115"/>
       <c r="B116" s="29" t="s">
         <v>221</v>
       </c>
@@ -4095,15 +4095,15 @@
       <c r="F116" s="29"/>
     </row>
     <row r="117" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="110"/>
-      <c r="B117" s="111"/>
-      <c r="C117" s="111"/>
-      <c r="D117" s="111"/>
-      <c r="E117" s="111"/>
-      <c r="F117" s="112"/>
+      <c r="A117" s="111"/>
+      <c r="B117" s="112"/>
+      <c r="C117" s="112"/>
+      <c r="D117" s="112"/>
+      <c r="E117" s="112"/>
+      <c r="F117" s="113"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="100" t="s">
+      <c r="A118" s="118" t="s">
         <v>117</v>
       </c>
       <c r="B118" s="13" t="s">
@@ -4121,7 +4121,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="100"/>
+      <c r="A119" s="118"/>
       <c r="B119" s="13" t="s">
         <v>46</v>
       </c>
@@ -4137,15 +4137,15 @@
       </c>
     </row>
     <row r="120" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="110"/>
-      <c r="B120" s="111"/>
-      <c r="C120" s="111"/>
-      <c r="D120" s="111"/>
-      <c r="E120" s="111"/>
-      <c r="F120" s="112"/>
+      <c r="A120" s="111"/>
+      <c r="B120" s="112"/>
+      <c r="C120" s="112"/>
+      <c r="D120" s="112"/>
+      <c r="E120" s="112"/>
+      <c r="F120" s="113"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="97" t="s">
+      <c r="A121" s="138" t="s">
         <v>43</v>
       </c>
       <c r="B121" s="15" t="s">
@@ -4163,7 +4163,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="97"/>
+      <c r="A122" s="138"/>
       <c r="B122" s="15" t="s">
         <v>46</v>
       </c>
@@ -4183,21 +4183,21 @@
       <c r="E123" s="6"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="96" t="s">
+      <c r="A124" s="91" t="s">
         <v>160</v>
       </c>
-      <c r="B124" s="96"/>
-      <c r="C124" s="96"/>
-      <c r="D124" s="96"/>
-      <c r="E124" s="96"/>
-      <c r="F124" s="96"/>
+      <c r="B124" s="91"/>
+      <c r="C124" s="91"/>
+      <c r="D124" s="91"/>
+      <c r="E124" s="91"/>
+      <c r="F124" s="91"/>
     </row>
     <row r="126" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="95"/>
-      <c r="B126" s="104"/>
-      <c r="C126" s="104"/>
-      <c r="D126" s="95"/>
-      <c r="E126" s="95"/>
+      <c r="A126" s="122"/>
+      <c r="B126" s="123"/>
+      <c r="C126" s="123"/>
+      <c r="D126" s="122"/>
+      <c r="E126" s="122"/>
     </row>
     <row r="127" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="73"/>
@@ -4210,118 +4210,118 @@
       <c r="A128" s="2"/>
       <c r="B128" s="55"/>
       <c r="C128" s="55"/>
-      <c r="D128" s="106"/>
-      <c r="E128" s="106"/>
+      <c r="D128" s="107"/>
+      <c r="E128" s="107"/>
     </row>
     <row r="129" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="55"/>
       <c r="C129" s="55"/>
-      <c r="D129" s="106"/>
-      <c r="E129" s="106"/>
+      <c r="D129" s="107"/>
+      <c r="E129" s="107"/>
     </row>
     <row r="130" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="76"/>
       <c r="C130" s="55"/>
-      <c r="D130" s="106"/>
-      <c r="E130" s="106"/>
+      <c r="D130" s="107"/>
+      <c r="E130" s="107"/>
     </row>
     <row r="131" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="55"/>
       <c r="C131" s="55"/>
-      <c r="D131" s="106"/>
-      <c r="E131" s="106"/>
+      <c r="D131" s="107"/>
+      <c r="E131" s="107"/>
     </row>
     <row r="132" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="55"/>
       <c r="C132" s="55"/>
-      <c r="D132" s="106"/>
-      <c r="E132" s="106"/>
+      <c r="D132" s="107"/>
+      <c r="E132" s="107"/>
     </row>
     <row r="133" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="55"/>
       <c r="C133" s="55"/>
-      <c r="D133" s="106"/>
-      <c r="E133" s="106"/>
+      <c r="D133" s="107"/>
+      <c r="E133" s="107"/>
     </row>
     <row r="134" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="55"/>
       <c r="C134" s="55"/>
-      <c r="D134" s="106"/>
-      <c r="E134" s="106"/>
+      <c r="D134" s="107"/>
+      <c r="E134" s="107"/>
     </row>
     <row r="135" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="55"/>
       <c r="C135" s="55"/>
-      <c r="D135" s="106"/>
-      <c r="E135" s="106"/>
+      <c r="D135" s="107"/>
+      <c r="E135" s="107"/>
     </row>
     <row r="136" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="55"/>
       <c r="C136" s="55"/>
-      <c r="D136" s="106"/>
-      <c r="E136" s="106"/>
+      <c r="D136" s="107"/>
+      <c r="E136" s="107"/>
     </row>
     <row r="137" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="55"/>
       <c r="C137" s="55"/>
-      <c r="D137" s="106"/>
-      <c r="E137" s="106"/>
+      <c r="D137" s="107"/>
+      <c r="E137" s="107"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="105"/>
-      <c r="B138" s="93"/>
-      <c r="C138" s="93"/>
-      <c r="D138" s="106"/>
-      <c r="E138" s="106"/>
+      <c r="A138" s="106"/>
+      <c r="B138" s="137"/>
+      <c r="C138" s="137"/>
+      <c r="D138" s="107"/>
+      <c r="E138" s="107"/>
     </row>
     <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="105"/>
-      <c r="B139" s="92"/>
-      <c r="C139" s="92"/>
-      <c r="D139" s="106"/>
-      <c r="E139" s="106"/>
+      <c r="A139" s="106"/>
+      <c r="B139" s="136"/>
+      <c r="C139" s="136"/>
+      <c r="D139" s="107"/>
+      <c r="E139" s="107"/>
     </row>
     <row r="140" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="55"/>
       <c r="C140" s="55"/>
-      <c r="D140" s="106"/>
-      <c r="E140" s="106"/>
+      <c r="D140" s="107"/>
+      <c r="E140" s="107"/>
     </row>
     <row r="141" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="55"/>
       <c r="C141" s="55"/>
-      <c r="D141" s="106"/>
-      <c r="E141" s="106"/>
+      <c r="D141" s="107"/>
+      <c r="E141" s="107"/>
     </row>
     <row r="142" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="55"/>
       <c r="C142" s="55"/>
-      <c r="D142" s="106"/>
-      <c r="E142" s="106"/>
+      <c r="D142" s="107"/>
+      <c r="E142" s="107"/>
     </row>
     <row r="143" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="55"/>
       <c r="C143" s="55"/>
-      <c r="D143" s="106"/>
-      <c r="E143" s="106"/>
+      <c r="D143" s="107"/>
+      <c r="E143" s="107"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
-      <c r="B144" s="80"/>
-      <c r="C144" s="80"/>
+      <c r="B144" s="124"/>
+      <c r="C144" s="124"/>
       <c r="D144" s="38"/>
       <c r="E144" s="38"/>
     </row>
@@ -4343,33 +4343,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A96:F96"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="E69:E74"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C69:C74"/>
-    <mergeCell ref="A80:A90"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="D128:D143"/>
-    <mergeCell ref="E128:E143"/>
-    <mergeCell ref="A109:F109"/>
-    <mergeCell ref="A117:F117"/>
-    <mergeCell ref="A120:F120"/>
-    <mergeCell ref="A114:F114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A99:A106"/>
-    <mergeCell ref="A110:A113"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A107:F107"/>
-    <mergeCell ref="A126:C126"/>
     <mergeCell ref="B144:C144"/>
     <mergeCell ref="A39:B43"/>
     <mergeCell ref="A45:C45"/>
@@ -4386,6 +4359,33 @@
     <mergeCell ref="D126:E126"/>
     <mergeCell ref="A124:F124"/>
     <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A99:A106"/>
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A107:F107"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="D128:D143"/>
+    <mergeCell ref="E128:E143"/>
+    <mergeCell ref="A109:F109"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="A120:F120"/>
+    <mergeCell ref="A114:F114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A96:F96"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="E69:E74"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="A80:A90"/>
+    <mergeCell ref="A92:A95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>